<commit_message>
Add ShowPartitions toggle to bika_setup
It doesn't remove 100% of the partitions UI, but the main front-end clutter is hidden.
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/demo/demo.xlsx
+++ b/bika/lims/setupdata/demo/demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="920" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="44" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="920" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -315,7 +315,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3393" uniqueCount="1576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3395" uniqueCount="1577">
   <si>
     <t>Instructions</t>
   </si>
@@ -4175,19 +4175,22 @@
     <t>Auto log off period (minutes)</t>
   </si>
   <si>
+    <t>ShowPartitions</t>
+  </si>
+  <si>
+    <t>Show Sample Partitions</t>
+  </si>
+  <si>
     <t>ShowPricing</t>
   </si>
   <si>
-    <t>Show pricing information</t>
+    <t>Show pricing</t>
   </si>
   <si>
     <t>Currency</t>
   </si>
   <si>
     <t>ZAR</t>
-  </si>
-  <si>
-    <t>Show pricing</t>
   </si>
   <si>
     <t>MemberDiscount</t>
@@ -5777,7 +5780,7 @@
   </sheetPr>
   <dimension ref="1:7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -23253,9 +23256,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -23332,62 +23335,62 @@
         <v>1288</v>
       </c>
       <c r="B7" s="112" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C7" s="132" t="s">
         <v>1289</v>
+      </c>
+      <c r="C7" s="133" t="n">
+        <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="8">
       <c r="A8" s="6" t="s">
-        <v>1286</v>
+        <v>1290</v>
       </c>
       <c r="B8" s="112" t="s">
         <v>1290</v>
       </c>
-      <c r="C8" s="133" t="n">
-        <v>0</v>
+      <c r="C8" s="132" t="s">
+        <v>1291</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="9">
       <c r="A9" s="6" t="s">
-        <v>1291</v>
+        <v>1288</v>
       </c>
       <c r="B9" s="112" t="s">
-        <v>1292</v>
-      </c>
-      <c r="C9" s="132" t="n">
-        <v>15</v>
+        <v>1289</v>
+      </c>
+      <c r="C9" s="133" t="n">
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="10">
       <c r="A10" s="6" t="s">
-        <v>1013</v>
+        <v>1292</v>
       </c>
       <c r="B10" s="112" t="s">
         <v>1293</v>
       </c>
       <c r="C10" s="132" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="11">
       <c r="A11" s="6" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B11" s="112" t="s">
         <v>1294</v>
       </c>
-      <c r="B11" s="112" t="s">
-        <v>1295</v>
-      </c>
       <c r="C11" s="132" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="12">
       <c r="A12" s="6" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B12" s="112" t="s">
         <v>1296</v>
-      </c>
-      <c r="B12" s="112" t="s">
-        <v>1297</v>
       </c>
       <c r="C12" s="132" t="n">
         <v>5</v>
@@ -23395,120 +23398,120 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="13">
       <c r="A13" s="6" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B13" s="112" t="s">
         <v>1298</v>
       </c>
-      <c r="B13" s="112" t="s">
-        <v>1299</v>
-      </c>
       <c r="C13" s="132" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="14">
       <c r="A14" s="6" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B14" s="112" t="s">
         <v>1300</v>
       </c>
-      <c r="B14" s="112" t="s">
-        <v>1301</v>
-      </c>
-      <c r="C14" s="132"/>
+      <c r="C14" s="132" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="15">
       <c r="A15" s="6" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B15" s="112" t="s">
         <v>1302</v>
       </c>
-      <c r="B15" s="112" t="s">
-        <v>1303</v>
-      </c>
-      <c r="C15" s="133" t="n">
-        <v>0</v>
-      </c>
+      <c r="C15" s="132"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="16">
       <c r="A16" s="6" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B16" s="112" t="s">
         <v>1304</v>
       </c>
-      <c r="B16" s="112" t="s">
+      <c r="C16" s="133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="17">
+      <c r="A17" s="6" t="s">
         <v>1305</v>
       </c>
-      <c r="C16" s="133" t="n">
+      <c r="B17" s="112" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C17" s="133" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24.5" outlineLevel="0" r="17">
-      <c r="A17" s="6" t="s">
-        <v>1306</v>
-      </c>
-      <c r="B17" s="112" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24.5" outlineLevel="0" r="18">
+      <c r="A18" s="6" t="s">
         <v>1307</v>
       </c>
-      <c r="C17" s="134" t="s">
+      <c r="B18" s="112" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C18" s="134" t="s">
         <v>967</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="18">
-      <c r="A18" s="6" t="s">
-        <v>1308</v>
-      </c>
-      <c r="B18" s="112" t="s">
-        <v>1309</v>
-      </c>
-      <c r="C18" s="135" t="s">
-        <v>1310</v>
-      </c>
-      <c r="D18" s="136"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="19">
       <c r="A19" s="6" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B19" s="112" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C19" s="135" t="s">
         <v>1311</v>
-      </c>
-      <c r="B19" s="112" t="s">
-        <v>1312</v>
-      </c>
-      <c r="C19" s="134" t="s">
-        <v>313</v>
       </c>
       <c r="D19" s="136"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="20">
       <c r="A20" s="6" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B20" s="112" t="s">
         <v>1313</v>
-      </c>
-      <c r="B20" s="112" t="s">
-        <v>1314</v>
       </c>
       <c r="C20" s="134" t="s">
         <v>313</v>
       </c>
+      <c r="D20" s="136"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="21">
       <c r="A21" s="6" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B21" s="112" t="s">
         <v>1315</v>
       </c>
-      <c r="B21" s="112" t="s">
-        <v>1316</v>
-      </c>
-      <c r="C21" s="135" t="n">
-        <v>30</v>
+      <c r="C21" s="134" t="s">
+        <v>313</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="22">
       <c r="A22" s="6" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B22" s="112" t="s">
         <v>1317</v>
       </c>
-      <c r="B22" s="112" t="s">
-        <v>1318</v>
-      </c>
       <c r="C22" s="135" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="23">
       <c r="A23" s="6" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B23" s="112" t="s">
         <v>1319</v>
-      </c>
-      <c r="B23" s="112" t="s">
-        <v>1320</v>
       </c>
       <c r="C23" s="135" t="n">
         <v>0</v>
@@ -23516,95 +23519,106 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="24">
       <c r="A24" s="6" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B24" s="112" t="s">
         <v>1321</v>
       </c>
-      <c r="B24" s="112" t="s">
-        <v>1322</v>
-      </c>
-      <c r="C24" s="134" t="s">
-        <v>1323</v>
-      </c>
-      <c r="D24" s="137"/>
+      <c r="C24" s="135" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="25">
       <c r="A25" s="6" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B25" s="112" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C25" s="134" t="s">
         <v>1324</v>
       </c>
-      <c r="B25" s="112" t="s">
+      <c r="D25" s="137"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="26">
+      <c r="A26" s="6" t="s">
         <v>1325</v>
       </c>
-      <c r="C25" s="134" t="s">
+      <c r="B26" s="112" t="s">
         <v>1326</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24.5" outlineLevel="0" r="26">
-      <c r="A26" s="6" t="s">
+      <c r="C26" s="134" t="s">
         <v>1327</v>
       </c>
-      <c r="B26" s="112" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24.5" outlineLevel="0" r="27">
+      <c r="A27" s="6" t="s">
         <v>1328</v>
       </c>
-      <c r="C26" s="133" t="n">
+      <c r="B27" s="112" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C27" s="133" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="27">
-      <c r="A27" s="6" t="s">
-        <v>1329</v>
-      </c>
-      <c r="B27" s="112" t="s">
-        <v>1330</v>
-      </c>
-      <c r="C27" s="132" t="s">
-        <v>1331</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="28">
       <c r="A28" s="6" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B28" s="112" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C28" s="132" t="s">
         <v>1332</v>
-      </c>
-      <c r="B28" s="112" t="s">
-        <v>1333</v>
-      </c>
-      <c r="C28" s="132" t="n">
-        <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="29">
       <c r="A29" s="6" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B29" s="112" t="s">
         <v>1334</v>
       </c>
-      <c r="B29" s="112" t="s">
-        <v>1335</v>
-      </c>
-      <c r="C29" s="133" t="n">
-        <v>0</v>
+      <c r="C29" s="132" t="n">
+        <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="30">
       <c r="A30" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B30" s="112" t="s">
         <v>1336</v>
       </c>
-      <c r="B30" s="112" t="s">
+      <c r="C30" s="133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="31">
+      <c r="A31" s="6" t="s">
         <v>1337</v>
       </c>
-      <c r="C30" s="132"/>
+      <c r="B31" s="112" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C31" s="132"/>
     </row>
   </sheetData>
   <dataValidations count="24">
-    <dataValidation allowBlank="true" error="Please enter a whole number bigger than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Please enter a whole number bigger than 0" promptTitle="Integer" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C21" type="whole">
+    <dataValidation allowBlank="true" error="Please enter a whole number bigger than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Please enter a whole number bigger than 0" promptTitle="Integer" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C22" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6 C8 C15:C16 C26 C29" type="list">
+    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6:C7 C9 C16:C17 C27 C30" type="list">
       <formula1>Constants!$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 23" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 23" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C22" type="whole">
+    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 23" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 23" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C23" type="whole">
       <formula1>0</formula1>
       <formula2>23</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 59" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 59" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C23" type="whole">
+    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 59" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 59" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C24" type="whole">
       <formula1>0</formula1>
       <formula2>59</formula2>
     </dataValidation>
@@ -23616,75 +23630,75 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Select a valid entry from the selection list" errorTitle="Invalid entry" operator="equal" prompt="Select a valid currency from the list. Currency codes are maintained on the &quot;Constants&quot; sheet" promptTitle="Currency code" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C7" type="list">
+    <dataValidation allowBlank="false" error="Select a valid entry from the selection list" errorTitle="Invalid entry" operator="equal" prompt="Select a valid currency from the list. Currency codes are maintained on the &quot;Constants&quot; sheet" promptTitle="Currency code" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C8" type="list">
       <formula1>Constants!$B$22:$B$200</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Not sure why, must be equal or greater than 0" errorTitle="Invalid entry" operator="between" prompt="The discount percentage entered here, is applied to the prices for clients flagged as 'members', normally co-operative members or associates deserving of this discount" promptTitle="Member discount %" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C9" type="decimal">
+    <dataValidation allowBlank="false" error="Not sure why, must be equal or greater than 0" errorTitle="Invalid entry" operator="between" prompt="The discount percentage entered here, is applied to the prices for clients flagged as 'members', normally co-operative members or associates deserving of this discount" promptTitle="Member discount %" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C10" type="decimal">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Not sure why, must be equal or greater than 0" errorTitle="Invalid entry" operator="between" prompt="Enter percentage value eg. 14.0.  This percentage is applied system-wide but can be overwrittem on individual items" promptTitle="Value added tax %" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C10" type="decimal">
+    <dataValidation allowBlank="true" error="Not sure why, must be equal or greater than 0" errorTitle="Invalid entry" operator="between" prompt="Enter percentage value eg. 14.0.  This percentage is applied system-wide but can be overwrittem on individual items" promptTitle="Value added tax %" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C11" type="decimal">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Using too few data points does not make statistical sense.  Set an acceptable minimum number of results before QC statistics will be calculated and plotted" promptTitle="Minimum number of results for QC stats calculations" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C11" type="whole">
+    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Using too few data points does not make statistical sense.  Set an acceptable minimum number of results before QC statistics will be calculated and plotted" promptTitle="Minimum number of results for QC stats calculations" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C12" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Set the maximum number of analysis requests per results email. Too many columns per email are difficult to read for some clients who prefer fewer results per email" promptTitle="Maximum columns per results email" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C12" type="whole">
+    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Set the maximum number of analysis requests per results email. Too many columns per email are difficult to read for some clients who prefer fewer results per email" promptTitle="Maximum columns per results email" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C13" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Too many AR columns per fax will see the font size minimised and could render faxes illegible. 4 ARs maximum per page is recommended" promptTitle="Maximum columns per results fax" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C13" type="whole">
+    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Too many AR columns per fax will see the font size minimised and could render faxes illegible. 4 ARs maximum per page is recommended" promptTitle="Maximum columns per results fax" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C14" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" prompt="The email to SMS gateway address. Either a complete email address, or just the domain, e.g. '@2way.co.za', the contact's mobile phone number will be prepended to" promptTitle="SMS Gateway Email Address" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C14" type="none">
+    <dataValidation allowBlank="true" operator="equal" prompt="The email to SMS gateway address. Either a complete email address, or just the domain, e.g. '@2way.co.za', the contact's mobile phone number will be prepended to" promptTitle="SMS Gateway Email Address" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C15" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The analysis to be used for determining dry matter. Please select a valid entry from the drop-down menu" promptTitle="Dry Matter Analysis" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C17" type="list">
+    <dataValidation allowBlank="true" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The analysis to be used for determining dry matter. Please select a valid entry from the drop-down menu" promptTitle="Dry Matter Analysis" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C18" type="list">
       <formula1>'Analysis Services'!$A$4:$A$167</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please selct a valid option from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The list is mainatined on the &quot;Constants&quot; sheet" promptTitle="Select an import format from the list" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C18" type="list">
+    <dataValidation allowBlank="false" error="Please selct a valid option from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The list is mainatined on the &quot;Constants&quot; sheet" promptTitle="Select an import format from the list" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C19" type="list">
       <formula1>Constants!$C$2:$C$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The analysis to be used for determining moisture. Please select a valid entry from the drop-down menu" promptTitle="Analysis keyword" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D18" type="list">
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The analysis to be used for determining moisture. Please select a valid entry from the drop-down menu" promptTitle="Analysis keyword" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D19" type="list">
       <formula1>'analysis services'</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Please select a valid option from the list" promptTitle="File attachments Required, Permitted or Not?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C19:C20" type="list">
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Please select a valid option from the list" promptTitle="File attachments Required, Permitted or Not?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C20:C21" type="list">
       <formula1>Constants!$D$2:$D$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="'Classic' indicates importing analysis requests per sample and analysis service selection. With 'Profiles', analysis profile keywords are used to select multiple analysis services together" promptTitle="AR Import options" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D19" type="list">
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="'Classic' indicates importing analysis requests per sample and analysis service selection. With 'Profiles', analysis profile keywords are used to select multiple analysis services together" promptTitle="AR Import options" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D20" type="list">
       <formula1>Constants!$B$2:$B$25</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 'Register' if you want labels to be automatically printed when new ARs or sample records are created. Select 'Receive' to print labels when ARs or Samples are received. Select 'None' to disable automatic printing" promptTitle="Select a valid option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C24" type="list">
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 'Register' if you want labels to be automatically printed when new ARs or sample records are created. Select 'Receive' to print labels when ARs or Samples are received. Select 'None' to disable automatic printing" promptTitle="Select a valid option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C25" type="list">
       <formula1>Constants!$F$2:$F$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The number of days before a sample expires and cannot be analysed any more. This setting can be overwritten per individual sample type  in the sample types setup" promptTitle="Default sample retention period" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D24" type="whole">
+    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The number of days before a sample expires and cannot be analysed any more. This setting can be overwritten per individual sample type  in the sample types setup" promptTitle="Default sample retention period" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D25" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select the which label to print when automatic label printing is enabled" promptTitle="Sample label size" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C25" type="list">
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select the which label to print when automatic label printing is enabled" promptTitle="Sample label size" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C26" type="list">
       <formula1>Constants!$E$2:$E$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The length of the zero-padding for Sample IDs. E.g, a water sample will be given an ID of W-0001 if the sample padding was set to 4, and water samples are prefixed with W" promptTitle="Sample ID Padding" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C27" type="whole">
+    <dataValidation allowBlank="false" error="Must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The length of the zero-padding for Sample IDs. E.g, a water sample will be given an ID of W-0001 if the sample padding was set to 4, and water samples are prefixed with W" promptTitle="Sample ID Padding" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C28" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The length of the zero-padding for AR IDs. E.g, a the first AR on a water sample with ID of W-0001 will be given an ID of W-0001-01 if the AR padding was set to 2" promptTitle="Analysis request (AR) ID Padding" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C28" type="whole">
+    <dataValidation allowBlank="false" error="Must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The length of the zero-padding for AR IDs. E.g, a the first AR on a water sample with ID of W-0001 will be given an ID of W-0001-01 if the AR padding was set to 2" promptTitle="Analysis request (AR) ID Padding" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C29" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The full URL: http://URL/path:port" promptTitle="ID Server URL if an external ID server is used" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C30" type="whole">
+    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The full URL: http://URL/path:port" promptTitle="ID Server URL if an external ID server is used" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C31" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -23733,28 +23747,28 @@
         <v>123</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="E1" s="72" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="F1" s="64" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="G1" s="140" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="H1" s="72" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="I1" s="72" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="J1" s="72" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="K1" s="72" t="s">
         <v>1024</v>
@@ -23763,22 +23777,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="2">
       <c r="A2" s="78" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="B2" s="78" t="s">
         <v>206</v>
       </c>
       <c r="C2" s="112" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D2" s="112" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="E2" s="138" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="F2" s="112" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="G2" s="112" t="n">
         <v>0</v>
@@ -23790,7 +23804,7 @@
         <v>1087</v>
       </c>
       <c r="J2" s="112" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="K2" s="112" t="s">
         <v>1039</v>
@@ -23798,34 +23812,34 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="3">
       <c r="A3" s="78" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="B3" s="78" t="s">
         <v>192</v>
       </c>
       <c r="C3" s="112" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D3" s="112" t="s">
         <v>313</v>
       </c>
       <c r="E3" s="138" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="F3" s="112" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="G3" s="112" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="112" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="I3" s="112" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="J3" s="112" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="K3" s="112" t="s">
         <v>1047</v>
@@ -23833,35 +23847,35 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="4">
       <c r="A4" s="78" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="B4" s="78" t="s">
         <v>152</v>
       </c>
       <c r="C4" s="112" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D4" s="112" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="F4" s="112" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="G4" s="138"/>
       <c r="H4" s="112" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="5">
       <c r="A5" s="112" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="B5" s="112" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="G5" s="138"/>
       <c r="H5" s="112" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="6">
@@ -23873,7 +23887,7 @@
       </c>
       <c r="G6" s="138"/>
       <c r="H6" s="112" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="7">
@@ -23881,16 +23895,16 @@
         <v>190</v>
       </c>
       <c r="B7" s="112" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="G7" s="138"/>
       <c r="H7" s="112" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="8">
       <c r="A8" s="78" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="B8" s="78" t="s">
         <v>214</v>
@@ -23946,39 +23960,39 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="58.45" outlineLevel="0" r="21" s="144">
       <c r="A21" s="64" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="B21" s="72" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
       <c r="C21" s="64" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D21" s="64" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="E21" s="143" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="F21" s="64" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="G21" s="64" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="H21" s="64" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="I21" s="64" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="22">
       <c r="A22" s="145" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="B22" s="112" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="C22" s="112" t="s">
         <v>1212</v>
@@ -23987,10 +24001,10 @@
         <v>1219</v>
       </c>
       <c r="E22" s="138" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="F22" s="112" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="G22" s="112" t="s">
         <v>919</v>
@@ -24004,19 +24018,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24.5" outlineLevel="0" r="23">
       <c r="B23" s="112" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="C23" s="112" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D23" s="112" t="s">
         <v>1260</v>
       </c>
       <c r="E23" s="138" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="F23" s="112" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="G23" s="112" t="s">
         <v>925</v>
@@ -24025,21 +24039,21 @@
         <v>925</v>
       </c>
       <c r="I23" s="112" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="24">
       <c r="B24" s="112" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="C24" s="112" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D24" s="112" t="s">
         <v>1262</v>
       </c>
       <c r="F24" s="112" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="G24" s="112" t="s">
         <v>922</v>
@@ -24048,926 +24062,926 @@
         <v>922</v>
       </c>
       <c r="I24" s="112" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="25">
       <c r="B25" s="112" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="C25" s="112" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D25" s="112" t="s">
         <v>1279</v>
       </c>
       <c r="H25" s="112" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="I25" s="112" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="26">
       <c r="B26" s="112" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="C26" s="112" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="H26" s="112" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="27">
       <c r="B27" s="112" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="C27" s="112" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="28">
       <c r="B28" s="112" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="C28" s="112" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="29">
       <c r="B29" s="112" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="C29" s="112" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="30">
       <c r="B30" s="112" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="C30" s="112" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="31">
       <c r="B31" s="112" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="C31" s="112" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="32">
       <c r="B32" s="112" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="C32" s="112" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="33">
       <c r="B33" s="112" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="C33" s="112" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="34">
       <c r="B34" s="112" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="35">
       <c r="B35" s="112" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="36">
       <c r="B36" s="112" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="37">
       <c r="B37" s="112" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="38">
       <c r="B38" s="112" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="39">
       <c r="B39" s="112" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="40">
       <c r="B40" s="112" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="41">
       <c r="B41" s="112" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="42">
       <c r="B42" s="112" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="43">
       <c r="B43" s="112" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="44">
       <c r="B44" s="112" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="45">
       <c r="B45" s="112" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="46">
       <c r="B46" s="112" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="47">
       <c r="B47" s="112" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="48">
       <c r="B48" s="112" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="49">
       <c r="B49" s="112" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="50">
       <c r="B50" s="112" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="51">
       <c r="B51" s="112" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="52">
       <c r="B52" s="112" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="53">
       <c r="B53" s="112" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="54">
       <c r="B54" s="112" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="55">
       <c r="B55" s="112" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="56">
       <c r="B56" s="112" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="57">
       <c r="B57" s="112" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="58">
       <c r="B58" s="112" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="59">
       <c r="B59" s="112" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="60">
       <c r="B60" s="112" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="61">
       <c r="B61" s="112" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="62">
       <c r="B62" s="112" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="63">
       <c r="B63" s="112" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="64">
       <c r="B64" s="112" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="65">
       <c r="B65" s="112" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="66">
       <c r="B66" s="112" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="67">
       <c r="B67" s="112" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="68">
       <c r="B68" s="112" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="69">
       <c r="B69" s="112" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="70">
       <c r="B70" s="112" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="71">
       <c r="B71" s="112" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="72">
       <c r="B72" s="112" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="73">
       <c r="B73" s="112" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="74">
       <c r="B74" s="112" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="75">
       <c r="B75" s="112" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="76">
       <c r="B76" s="112" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="77">
       <c r="B77" s="112" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="78">
       <c r="B78" s="112" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="79">
       <c r="B79" s="112" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="80">
       <c r="B80" s="112" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="81">
       <c r="B81" s="112" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="82">
       <c r="B82" s="112" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="83">
       <c r="B83" s="112" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="84">
       <c r="B84" s="112" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="85">
       <c r="B85" s="112" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="86">
       <c r="B86" s="112" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="87">
       <c r="B87" s="112" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="88">
       <c r="B88" s="112" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="89">
       <c r="B89" s="112" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="90">
       <c r="B90" s="112" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="91">
       <c r="B91" s="112" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="92">
       <c r="B92" s="112" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="93">
       <c r="B93" s="112" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="94">
       <c r="B94" s="112" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="95">
       <c r="B95" s="112" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="96">
       <c r="B96" s="112" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="97">
       <c r="B97" s="112" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="98">
       <c r="B98" s="112" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="99">
       <c r="B99" s="112" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="100">
       <c r="B100" s="112" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="101">
       <c r="B101" s="112" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="102">
       <c r="B102" s="112" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="103">
       <c r="B103" s="112" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="104">
       <c r="B104" s="112" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="105">
       <c r="B105" s="112" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="106">
       <c r="B106" s="112" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="107">
       <c r="B107" s="112" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="108">
       <c r="B108" s="112" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="109">
       <c r="B109" s="112" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="110">
       <c r="B110" s="112" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="111">
       <c r="B111" s="112" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="112">
       <c r="B112" s="112" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="113">
       <c r="B113" s="112" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="114">
       <c r="B114" s="112" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="115">
       <c r="B115" s="112" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="116">
       <c r="B116" s="112" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="117">
       <c r="B117" s="112" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="118">
       <c r="B118" s="112" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="119">
       <c r="B119" s="112" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="120">
       <c r="B120" s="112" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="121">
       <c r="B121" s="112" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="122">
       <c r="B122" s="112" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="123">
       <c r="B123" s="112" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="124">
       <c r="B124" s="112" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="125">
       <c r="B125" s="112" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="126">
       <c r="B126" s="112" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="127">
       <c r="B127" s="112" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="128">
       <c r="B128" s="112" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="129">
       <c r="B129" s="112" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="130">
       <c r="B130" s="112" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="131">
       <c r="B131" s="112" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="132">
       <c r="B132" s="112" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="133">
       <c r="B133" s="112" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="134">
       <c r="B134" s="112" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="135">
       <c r="B135" s="112" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="136">
       <c r="B136" s="112" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="137">
       <c r="B137" s="112" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="138">
       <c r="B138" s="112" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="139">
       <c r="B139" s="112" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="140">
       <c r="B140" s="112" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="141">
       <c r="B141" s="112" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="142">
       <c r="B142" s="112" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="143">
       <c r="B143" s="112" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="144">
       <c r="B144" s="112" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="145">
       <c r="B145" s="112" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="146">
       <c r="B146" s="112" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="147">
       <c r="B147" s="112" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="148">
       <c r="B148" s="112" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="149">
       <c r="B149" s="112" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="150">
       <c r="B150" s="112" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="151">
       <c r="B151" s="112" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="152">
       <c r="B152" s="112" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="153">
       <c r="B153" s="112" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="154">
       <c r="B154" s="112" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="155">
       <c r="B155" s="112" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="156">
       <c r="B156" s="112" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="157">
       <c r="B157" s="112" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="158">
       <c r="B158" s="112" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="159">
       <c r="B159" s="112" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="160">
       <c r="B160" s="112" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="161">
       <c r="B161" s="112" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="162">
       <c r="B162" s="112" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="163">
       <c r="B163" s="112" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="164">
       <c r="B164" s="112" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="165">
       <c r="B165" s="112" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="166">
       <c r="B166" s="112" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="167">
       <c r="B167" s="112" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="168">
       <c r="B168" s="112" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="169">
       <c r="B169" s="112" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="170">
       <c r="B170" s="112" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="171">
       <c r="B171" s="112" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="172">
       <c r="B172" s="112" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="173">
       <c r="B173" s="112" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="174">
       <c r="B174" s="112" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="175">
       <c r="B175" s="112" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="176">
       <c r="B176" s="112" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="177">
       <c r="B177" s="112" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="178">
       <c r="B178" s="112" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="179">
       <c r="B179" s="112" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="180">
       <c r="B180" s="112" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="181">
       <c r="B181" s="112" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="182">
       <c r="B182" s="112" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="183">
       <c r="B183" s="112" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="184">
       <c r="B184" s="112" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="185">
       <c r="B185" s="112" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="186">
       <c r="B186" s="112" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="187">
       <c r="B187" s="112" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="188">
       <c r="B188" s="112" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="189">
       <c r="B189" s="112" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="190">
       <c r="B190" s="112" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="191">
       <c r="B191" s="112" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="192">
       <c r="B192" s="112" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="193">
       <c r="B193" s="112" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="194">
       <c r="B194" s="112" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="195">
       <c r="B195" s="112" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="196">
       <c r="B196" s="112" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="197">
       <c r="B197" s="112" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="198">
       <c r="B198" s="112" t="s">
-        <v>1289</v>
+        <v>1291</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="199">
       <c r="B199" s="112" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="200">
       <c r="B200" s="112" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>